<commit_message>
Cambio tipo de sueldo, fecha de baja, vencimiento contrato
</commit_message>
<xml_diff>
--- a/Payroll/Content/Download/CargaMasiva.xlsx
+++ b/Payroll/Content/Download/CargaMasiva.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marco Carranza\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marco Carranza\Documents\IPSNET-Nomina\developeraguilar\Seri\Payroll\Content\Download\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF65FB8D-A30F-4B1F-9444-B3C4DC976172}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{806648D8-EFDA-4C29-B944-0459F192E4BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="12" activeTab="15" xr2:uid="{B7450375-384B-4A8B-AB27-614585F29454}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{B7450375-384B-4A8B-AB27-614585F29454}"/>
   </bookViews>
   <sheets>
     <sheet name="IPSNet Cargas" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="507">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="508">
   <si>
     <t>DATA</t>
   </si>
@@ -1561,6 +1561,9 @@
   </si>
   <si>
     <t>N/A</t>
+  </si>
+  <si>
+    <t>TipoSueldo</t>
   </si>
 </sst>
 </file>
@@ -1956,10 +1959,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A634B92-38F3-48BB-89EF-6C7BAE71E424}">
-  <dimension ref="A1:AS7"/>
+  <dimension ref="A1:AT7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AS2" sqref="AS2"/>
+    <sheetView tabSelected="1" topLeftCell="AH1" workbookViewId="0">
+      <selection activeCell="AT1" sqref="AT1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1983,7 +1986,7 @@
     <col min="44" max="44" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A1" s="3">
         <v>2</v>
       </c>
@@ -2119,8 +2122,11 @@
       <c r="AS1" s="8" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="2" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AT1" s="8" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
       <c r="D2">
         <v>4</v>
       </c>
@@ -2241,8 +2247,11 @@
       <c r="AS2">
         <v>27677</v>
       </c>
-    </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AT2">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
       <c r="D3">
         <v>4</v>
       </c>
@@ -2363,8 +2372,11 @@
       <c r="AS3">
         <v>2531932</v>
       </c>
-    </row>
-    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AT3">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="7" spans="1:46" x14ac:dyDescent="0.25">
       <c r="AB7" t="s">
         <v>52</v>
       </c>
@@ -2781,7 +2793,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00E05364-4ABD-4239-B4EA-F0FE2D369467}">
   <dimension ref="A1:B95"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D1" activeCellId="1" sqref="C1:C1048576 D1:D1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Correciones apartado de los empleados, campos en historial, validacion longitud de cuentas, mostrar boton de guardar registro al momento de limpiar locsto
</commit_message>
<xml_diff>
--- a/Payroll/Content/Download/CargaMasiva.xlsx
+++ b/Payroll/Content/Download/CargaMasiva.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marco Carranza\Documents\IPSNET-Nomina\developeraguilar\Seri\Payroll\Content\Download\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marco Carranza\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{806648D8-EFDA-4C29-B944-0459F192E4BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7063EDA7-32A2-4112-930D-44188EA3FBF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{B7450375-384B-4A8B-AB27-614585F29454}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="508">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="513">
   <si>
     <t>DATA</t>
   </si>
@@ -48,18 +48,9 @@
     <t>MassiveLoads</t>
   </si>
   <si>
-    <t>Jose</t>
-  </si>
-  <si>
     <t>Carlos</t>
   </si>
   <si>
-    <t>Martinez</t>
-  </si>
-  <si>
-    <t>Gomez</t>
-  </si>
-  <si>
     <t>Cardenas</t>
   </si>
   <si>
@@ -1563,14 +1554,38 @@
     <t>N/A</t>
   </si>
   <si>
-    <t>TipoSueldo</t>
+    <t>Tipo salario</t>
+  </si>
+  <si>
+    <t>Politica</t>
+  </si>
+  <si>
+    <t>Diferencia P</t>
+  </si>
+  <si>
+    <t>Transporte</t>
+  </si>
+  <si>
+    <t>gf</t>
+  </si>
+  <si>
+    <t>Marco</t>
+  </si>
+  <si>
+    <t>Carranza</t>
+  </si>
+  <si>
+    <t>Aguilar</t>
+  </si>
+  <si>
+    <t>28-08-1997</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1582,6 +1597,13 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1628,13 +1650,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1644,10 +1666,13 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Porcentaje" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1959,10 +1984,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A634B92-38F3-48BB-89EF-6C7BAE71E424}">
-  <dimension ref="A1:AT7"/>
+  <dimension ref="A1:AW7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AH1" workbookViewId="0">
-      <selection activeCell="AT1" sqref="AT1"/>
+    <sheetView tabSelected="1" topLeftCell="AJ1" workbookViewId="0">
+      <selection activeCell="AU9" sqref="AU9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1986,164 +2011,173 @@
     <col min="44" max="44" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A1" s="3">
+    <row r="1" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="A1" s="2">
         <v>2</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="L1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="M1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="N1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="O1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="P1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="Q1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="R1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="P1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="S1" s="2" t="s">
+      <c r="S1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="V1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="W1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="U1" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="W1" s="2" t="s">
+      <c r="X1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Y1" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="Y1" s="7" t="s">
+      <c r="Z1" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA1" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB1" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="Z1" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="AA1" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="AB1" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AC1" s="7" t="s">
+      <c r="AC1" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="AD1" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="AE1" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="AD1" s="7" t="s">
+      <c r="AF1" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="AE1" s="8" t="s">
+      <c r="AG1" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="AH1" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="AF1" s="8" t="s">
+      <c r="AI1" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="AG1" s="8" t="s">
+      <c r="AJ1" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="AH1" s="8" t="s">
+      <c r="AK1" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="AI1" s="8" t="s">
+      <c r="AL1" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="AJ1" s="8" t="s">
+      <c r="AM1" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="AK1" s="8" t="s">
+      <c r="AN1" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="AL1" s="8" t="s">
+      <c r="AO1" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="AM1" s="8" t="s">
+      <c r="AP1" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="AN1" s="8" t="s">
+      <c r="AQ1" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="AO1" s="8" t="s">
+      <c r="AR1" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="AP1" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="AQ1" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="AR1" s="8" t="s">
+      <c r="AS1" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="AS1" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="AT1" s="8" t="s">
+      <c r="AT1" s="7" t="s">
+        <v>504</v>
+      </c>
+      <c r="AU1" s="7" t="s">
+        <v>505</v>
+      </c>
+      <c r="AV1" s="7" t="s">
+        <v>506</v>
+      </c>
+      <c r="AW1" s="7" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:49" x14ac:dyDescent="0.25">
       <c r="D2">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>2</v>
+        <v>509</v>
       </c>
       <c r="F2" t="s">
-        <v>4</v>
+        <v>510</v>
       </c>
       <c r="G2" t="s">
+        <v>511</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>512</v>
+      </c>
+      <c r="I2" t="s">
         <v>5</v>
-      </c>
-      <c r="H2" s="1">
-        <v>32883</v>
-      </c>
-      <c r="I2" t="s">
-        <v>8</v>
       </c>
       <c r="J2">
         <v>62</v>
@@ -2164,13 +2198,13 @@
         <v>12</v>
       </c>
       <c r="P2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="Q2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="R2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="S2">
         <v>99</v>
@@ -2178,26 +2212,26 @@
       <c r="U2">
         <v>9872637182</v>
       </c>
-      <c r="V2" s="5" t="s">
+      <c r="V2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="W2" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="X2" t="s">
         <v>36</v>
       </c>
-      <c r="W2" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="X2" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y2" s="6" t="s">
-        <v>45</v>
+      <c r="Y2" s="5" t="s">
+        <v>42</v>
       </c>
       <c r="Z2">
         <v>66878989878</v>
       </c>
-      <c r="AA2" s="6" t="s">
-        <v>47</v>
+      <c r="AA2" s="5" t="s">
+        <v>44</v>
       </c>
       <c r="AB2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="AC2">
         <v>199</v>
@@ -2205,8 +2239,8 @@
       <c r="AD2">
         <v>70</v>
       </c>
-      <c r="AE2" s="6" t="s">
-        <v>45</v>
+      <c r="AE2" s="5" t="s">
+        <v>42</v>
       </c>
       <c r="AF2">
         <v>4500.4799999999996</v>
@@ -2229,11 +2263,11 @@
       <c r="AL2">
         <v>140</v>
       </c>
-      <c r="AM2" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="AN2" s="6" t="s">
-        <v>45</v>
+      <c r="AM2" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="AN2" s="5" t="s">
+        <v>42</v>
       </c>
       <c r="AP2">
         <v>221</v>
@@ -2241,8 +2275,8 @@
       <c r="AQ2">
         <v>14</v>
       </c>
-      <c r="AR2" s="6" t="s">
-        <v>67</v>
+      <c r="AR2" s="5" t="s">
+        <v>64</v>
       </c>
       <c r="AS2">
         <v>27677</v>
@@ -2250,25 +2284,34 @@
       <c r="AT2">
         <v>321</v>
       </c>
-    </row>
-    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AU2">
+        <v>1</v>
+      </c>
+      <c r="AV2">
+        <v>35.78</v>
+      </c>
+      <c r="AW2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:49" x14ac:dyDescent="0.25">
       <c r="D3">
+        <v>18</v>
+      </c>
+      <c r="E3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" t="s">
         <v>4</v>
       </c>
-      <c r="E3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" t="s">
         <v>6</v>
-      </c>
-      <c r="G3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I3" t="s">
-        <v>9</v>
       </c>
       <c r="J3">
         <v>622</v>
@@ -2289,13 +2332,13 @@
         <v>34</v>
       </c>
       <c r="P3" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q3" t="s">
         <v>26</v>
       </c>
-      <c r="Q3" t="s">
-        <v>29</v>
-      </c>
       <c r="R3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="S3">
         <v>72</v>
@@ -2307,22 +2350,22 @@
         <v>98765678987</v>
       </c>
       <c r="W3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="X3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="Y3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="Z3">
         <v>8989898989</v>
       </c>
-      <c r="AA3" s="6" t="s">
-        <v>48</v>
+      <c r="AA3" s="5" t="s">
+        <v>45</v>
       </c>
       <c r="AB3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="AC3">
         <v>215</v>
@@ -2330,8 +2373,8 @@
       <c r="AD3">
         <v>199</v>
       </c>
-      <c r="AE3" s="6" t="s">
-        <v>46</v>
+      <c r="AE3" s="5" t="s">
+        <v>43</v>
       </c>
       <c r="AF3">
         <v>8600</v>
@@ -2354,11 +2397,11 @@
       <c r="AL3">
         <v>140</v>
       </c>
-      <c r="AM3" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="AN3" s="6" t="s">
-        <v>45</v>
+      <c r="AM3" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="AN3" s="5" t="s">
+        <v>42</v>
       </c>
       <c r="AP3">
         <v>219</v>
@@ -2366,7 +2409,7 @@
       <c r="AQ3">
         <v>14</v>
       </c>
-      <c r="AR3" s="6">
+      <c r="AR3" s="5">
         <v>98989898988</v>
       </c>
       <c r="AS3">
@@ -2375,10 +2418,17 @@
       <c r="AT3">
         <v>345</v>
       </c>
-    </row>
-    <row r="7" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AU3">
+        <v>3</v>
+      </c>
+      <c r="AV3" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="7" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="H7" s="8"/>
       <c r="AB7" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -2401,10 +2451,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="B1" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -2412,7 +2462,7 @@
         <v>75</v>
       </c>
       <c r="B2" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2420,7 +2470,7 @@
         <v>76</v>
       </c>
       <c r="B3" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2428,7 +2478,7 @@
         <v>77</v>
       </c>
       <c r="B4" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -2436,7 +2486,7 @@
         <v>155</v>
       </c>
       <c r="B5" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -2444,7 +2494,7 @@
         <v>156</v>
       </c>
       <c r="B6" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
     </row>
   </sheetData>
@@ -2464,10 +2514,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="B1" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -2475,7 +2525,7 @@
         <v>72</v>
       </c>
       <c r="B2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2483,7 +2533,7 @@
         <v>73</v>
       </c>
       <c r="B3" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2491,7 +2541,7 @@
         <v>74</v>
       </c>
       <c r="B4" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
     </row>
   </sheetData>
@@ -2511,10 +2561,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="B1" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -2522,7 +2572,7 @@
         <v>80</v>
       </c>
       <c r="B2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2530,7 +2580,7 @@
         <v>81</v>
       </c>
       <c r="B3" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2538,7 +2588,7 @@
         <v>82</v>
       </c>
       <c r="B4" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -2546,7 +2596,7 @@
         <v>83</v>
       </c>
       <c r="B5" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
     </row>
   </sheetData>
@@ -2569,10 +2619,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="B1" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -2580,7 +2630,7 @@
         <v>89</v>
       </c>
       <c r="B2" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2588,7 +2638,7 @@
         <v>90</v>
       </c>
       <c r="B3" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2596,7 +2646,7 @@
         <v>91</v>
       </c>
       <c r="B4" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -2604,7 +2654,7 @@
         <v>92</v>
       </c>
       <c r="B5" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -2612,7 +2662,7 @@
         <v>93</v>
       </c>
       <c r="B6" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -2620,7 +2670,7 @@
         <v>94</v>
       </c>
       <c r="B7" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -2628,7 +2678,7 @@
         <v>95</v>
       </c>
       <c r="B8" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -2636,7 +2686,7 @@
         <v>96</v>
       </c>
       <c r="B9" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -2644,7 +2694,7 @@
         <v>97</v>
       </c>
       <c r="B10" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -2652,7 +2702,7 @@
         <v>98</v>
       </c>
       <c r="B11" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -2660,7 +2710,7 @@
         <v>99</v>
       </c>
       <c r="B12" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
     </row>
   </sheetData>
@@ -2680,10 +2730,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="B1" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -2691,7 +2741,7 @@
         <v>140</v>
       </c>
       <c r="B2" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2699,7 +2749,7 @@
         <v>141</v>
       </c>
       <c r="B3" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2707,7 +2757,7 @@
         <v>142</v>
       </c>
       <c r="B4" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -2715,7 +2765,7 @@
         <v>150</v>
       </c>
       <c r="B5" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -2723,7 +2773,7 @@
         <v>283</v>
       </c>
       <c r="B6" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
     </row>
   </sheetData>
@@ -2746,10 +2796,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="B1" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -2757,7 +2807,7 @@
         <v>218</v>
       </c>
       <c r="B2" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2765,7 +2815,7 @@
         <v>219</v>
       </c>
       <c r="B3" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2773,7 +2823,7 @@
         <v>220</v>
       </c>
       <c r="B4" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -2781,7 +2831,7 @@
         <v>221</v>
       </c>
       <c r="B5" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
     </row>
   </sheetData>
@@ -2801,10 +2851,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="B1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -2812,7 +2862,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2820,7 +2870,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2828,7 +2878,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -2836,7 +2886,7 @@
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -2844,7 +2894,7 @@
         <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -2852,7 +2902,7 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -2860,7 +2910,7 @@
         <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -2868,7 +2918,7 @@
         <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -2876,7 +2926,7 @@
         <v>30</v>
       </c>
       <c r="B10" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -2884,7 +2934,7 @@
         <v>32</v>
       </c>
       <c r="B11" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -2892,7 +2942,7 @@
         <v>36</v>
       </c>
       <c r="B12" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -2900,7 +2950,7 @@
         <v>37</v>
       </c>
       <c r="B13" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -2908,7 +2958,7 @@
         <v>42</v>
       </c>
       <c r="B14" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -2916,7 +2966,7 @@
         <v>44</v>
       </c>
       <c r="B15" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -2924,7 +2974,7 @@
         <v>58</v>
       </c>
       <c r="B16" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -2932,7 +2982,7 @@
         <v>59</v>
       </c>
       <c r="B17" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -2940,7 +2990,7 @@
         <v>60</v>
       </c>
       <c r="B18" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -2948,7 +2998,7 @@
         <v>62</v>
       </c>
       <c r="B19" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -2956,7 +3006,7 @@
         <v>72</v>
       </c>
       <c r="B20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -2964,7 +3014,7 @@
         <v>102</v>
       </c>
       <c r="B21" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -2972,7 +3022,7 @@
         <v>103</v>
       </c>
       <c r="B22" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -2980,7 +3030,7 @@
         <v>106</v>
       </c>
       <c r="B23" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -2988,7 +3038,7 @@
         <v>108</v>
       </c>
       <c r="B24" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -2996,7 +3046,7 @@
         <v>110</v>
       </c>
       <c r="B25" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -3004,7 +3054,7 @@
         <v>112</v>
       </c>
       <c r="B26" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -3012,7 +3062,7 @@
         <v>113</v>
       </c>
       <c r="B27" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -3020,7 +3070,7 @@
         <v>116</v>
       </c>
       <c r="B28" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -3028,7 +3078,7 @@
         <v>124</v>
       </c>
       <c r="B29" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -3036,7 +3086,7 @@
         <v>126</v>
       </c>
       <c r="B30" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -3044,7 +3094,7 @@
         <v>127</v>
       </c>
       <c r="B31" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -3052,7 +3102,7 @@
         <v>128</v>
       </c>
       <c r="B32" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -3060,7 +3110,7 @@
         <v>129</v>
       </c>
       <c r="B33" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -3068,7 +3118,7 @@
         <v>130</v>
       </c>
       <c r="B34" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -3076,7 +3126,7 @@
         <v>131</v>
       </c>
       <c r="B35" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -3084,7 +3134,7 @@
         <v>132</v>
       </c>
       <c r="B36" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -3092,7 +3142,7 @@
         <v>133</v>
       </c>
       <c r="B37" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -3100,7 +3150,7 @@
         <v>134</v>
       </c>
       <c r="B38" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -3108,7 +3158,7 @@
         <v>135</v>
       </c>
       <c r="B39" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -3116,7 +3166,7 @@
         <v>136</v>
       </c>
       <c r="B40" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -3124,7 +3174,7 @@
         <v>137</v>
       </c>
       <c r="B41" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -3132,7 +3182,7 @@
         <v>138</v>
       </c>
       <c r="B42" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -3140,7 +3190,7 @@
         <v>139</v>
       </c>
       <c r="B43" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -3148,7 +3198,7 @@
         <v>140</v>
       </c>
       <c r="B44" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -3156,7 +3206,7 @@
         <v>141</v>
       </c>
       <c r="B45" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -3164,7 +3214,7 @@
         <v>143</v>
       </c>
       <c r="B46" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -3172,7 +3222,7 @@
         <v>145</v>
       </c>
       <c r="B47" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -3180,7 +3230,7 @@
         <v>166</v>
       </c>
       <c r="B48" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -3188,7 +3238,7 @@
         <v>168</v>
       </c>
       <c r="B49" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -3196,7 +3246,7 @@
         <v>600</v>
       </c>
       <c r="B50" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -3204,7 +3254,7 @@
         <v>601</v>
       </c>
       <c r="B51" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -3212,7 +3262,7 @@
         <v>602</v>
       </c>
       <c r="B52" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -3220,7 +3270,7 @@
         <v>605</v>
       </c>
       <c r="B53" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -3228,7 +3278,7 @@
         <v>606</v>
       </c>
       <c r="B54" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -3236,7 +3286,7 @@
         <v>607</v>
       </c>
       <c r="B55" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -3244,7 +3294,7 @@
         <v>608</v>
       </c>
       <c r="B56" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -3252,7 +3302,7 @@
         <v>610</v>
       </c>
       <c r="B57" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -3260,7 +3310,7 @@
         <v>614</v>
       </c>
       <c r="B58" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -3268,7 +3318,7 @@
         <v>615</v>
       </c>
       <c r="B59" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -3276,7 +3326,7 @@
         <v>616</v>
       </c>
       <c r="B60" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -3284,7 +3334,7 @@
         <v>617</v>
       </c>
       <c r="B61" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
@@ -3292,7 +3342,7 @@
         <v>618</v>
       </c>
       <c r="B62" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -3300,7 +3350,7 @@
         <v>619</v>
       </c>
       <c r="B63" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -3308,7 +3358,7 @@
         <v>620</v>
       </c>
       <c r="B64" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -3316,7 +3366,7 @@
         <v>621</v>
       </c>
       <c r="B65" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
@@ -3324,7 +3374,7 @@
         <v>622</v>
       </c>
       <c r="B66" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
@@ -3332,7 +3382,7 @@
         <v>623</v>
       </c>
       <c r="B67" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
@@ -3340,7 +3390,7 @@
         <v>626</v>
       </c>
       <c r="B68" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
@@ -3348,7 +3398,7 @@
         <v>627</v>
       </c>
       <c r="B69" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
@@ -3356,7 +3406,7 @@
         <v>628</v>
       </c>
       <c r="B70" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
@@ -3364,7 +3414,7 @@
         <v>629</v>
       </c>
       <c r="B71" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
@@ -3372,7 +3422,7 @@
         <v>630</v>
       </c>
       <c r="B72" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
@@ -3380,7 +3430,7 @@
         <v>631</v>
       </c>
       <c r="B73" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
@@ -3388,7 +3438,7 @@
         <v>632</v>
       </c>
       <c r="B74" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
@@ -3396,7 +3446,7 @@
         <v>633</v>
       </c>
       <c r="B75" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
@@ -3404,7 +3454,7 @@
         <v>634</v>
       </c>
       <c r="B76" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
@@ -3412,7 +3462,7 @@
         <v>636</v>
       </c>
       <c r="B77" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
@@ -3420,7 +3470,7 @@
         <v>637</v>
       </c>
       <c r="B78" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
@@ -3428,7 +3478,7 @@
         <v>638</v>
       </c>
       <c r="B79" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
@@ -3436,7 +3486,7 @@
         <v>640</v>
       </c>
       <c r="B80" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
@@ -3444,7 +3494,7 @@
         <v>642</v>
       </c>
       <c r="B81" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
@@ -3452,7 +3502,7 @@
         <v>646</v>
       </c>
       <c r="B82" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
@@ -3460,7 +3510,7 @@
         <v>647</v>
       </c>
       <c r="B83" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
@@ -3468,7 +3518,7 @@
         <v>648</v>
       </c>
       <c r="B84" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
@@ -3476,7 +3526,7 @@
         <v>649</v>
       </c>
       <c r="B85" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
@@ -3484,7 +3534,7 @@
         <v>651</v>
       </c>
       <c r="B86" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
@@ -3492,7 +3542,7 @@
         <v>652</v>
       </c>
       <c r="B87" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
@@ -3500,7 +3550,7 @@
         <v>653</v>
       </c>
       <c r="B88" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
@@ -3508,7 +3558,7 @@
         <v>655</v>
       </c>
       <c r="B89" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
@@ -3516,7 +3566,7 @@
         <v>656</v>
       </c>
       <c r="B90" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
@@ -3524,7 +3574,7 @@
         <v>659</v>
       </c>
       <c r="B91" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
@@ -3532,7 +3582,7 @@
         <v>670</v>
       </c>
       <c r="B92" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
@@ -3540,7 +3590,7 @@
         <v>901</v>
       </c>
       <c r="B93" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
@@ -3548,7 +3598,7 @@
         <v>902</v>
       </c>
       <c r="B94" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
@@ -3556,7 +3606,7 @@
         <v>999</v>
       </c>
       <c r="B95" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
     </row>
   </sheetData>
@@ -3580,10 +3630,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -3591,7 +3641,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -3599,7 +3649,7 @@
         <v>100</v>
       </c>
       <c r="B3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -3607,7 +3657,7 @@
         <v>104</v>
       </c>
       <c r="B4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -3615,7 +3665,7 @@
         <v>108</v>
       </c>
       <c r="B5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -3623,7 +3673,7 @@
         <v>112</v>
       </c>
       <c r="B6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -3631,7 +3681,7 @@
         <v>116</v>
       </c>
       <c r="B7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -3639,7 +3689,7 @@
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -3647,7 +3697,7 @@
         <v>120</v>
       </c>
       <c r="B9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -3655,7 +3705,7 @@
         <v>124</v>
       </c>
       <c r="B10" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -3663,7 +3713,7 @@
         <v>132</v>
       </c>
       <c r="B11" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -3671,7 +3721,7 @@
         <v>136</v>
       </c>
       <c r="B12" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -3679,7 +3729,7 @@
         <v>140</v>
       </c>
       <c r="B13" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -3687,7 +3737,7 @@
         <v>144</v>
       </c>
       <c r="B14" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -3695,7 +3745,7 @@
         <v>148</v>
       </c>
       <c r="B15" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -3703,7 +3753,7 @@
         <v>152</v>
       </c>
       <c r="B16" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -3711,7 +3761,7 @@
         <v>156</v>
       </c>
       <c r="B17" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -3719,7 +3769,7 @@
         <v>158</v>
       </c>
       <c r="B18" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -3727,7 +3777,7 @@
         <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -3735,7 +3785,7 @@
         <v>162</v>
       </c>
       <c r="B20" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -3743,7 +3793,7 @@
         <v>166</v>
       </c>
       <c r="B21" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -3751,7 +3801,7 @@
         <v>170</v>
       </c>
       <c r="B22" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -3759,7 +3809,7 @@
         <v>174</v>
       </c>
       <c r="B23" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -3767,7 +3817,7 @@
         <v>175</v>
       </c>
       <c r="B24" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -3775,7 +3825,7 @@
         <v>178</v>
       </c>
       <c r="B25" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -3783,7 +3833,7 @@
         <v>180</v>
       </c>
       <c r="B26" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -3791,7 +3841,7 @@
         <v>184</v>
       </c>
       <c r="B27" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -3799,7 +3849,7 @@
         <v>188</v>
       </c>
       <c r="B28" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -3807,7 +3857,7 @@
         <v>191</v>
       </c>
       <c r="B29" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -3815,7 +3865,7 @@
         <v>192</v>
       </c>
       <c r="B30" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -3823,7 +3873,7 @@
         <v>196</v>
       </c>
       <c r="B31" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -3831,7 +3881,7 @@
         <v>20</v>
       </c>
       <c r="B32" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -3839,7 +3889,7 @@
         <v>203</v>
       </c>
       <c r="B33" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -3847,7 +3897,7 @@
         <v>204</v>
       </c>
       <c r="B34" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -3855,7 +3905,7 @@
         <v>208</v>
       </c>
       <c r="B35" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -3863,7 +3913,7 @@
         <v>212</v>
       </c>
       <c r="B36" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -3871,7 +3921,7 @@
         <v>214</v>
       </c>
       <c r="B37" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -3879,7 +3929,7 @@
         <v>218</v>
       </c>
       <c r="B38" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -3887,7 +3937,7 @@
         <v>222</v>
       </c>
       <c r="B39" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -3895,7 +3945,7 @@
         <v>226</v>
       </c>
       <c r="B40" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -3903,7 +3953,7 @@
         <v>231</v>
       </c>
       <c r="B41" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -3911,7 +3961,7 @@
         <v>232</v>
       </c>
       <c r="B42" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -3919,7 +3969,7 @@
         <v>233</v>
       </c>
       <c r="B43" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -3927,7 +3977,7 @@
         <v>234</v>
       </c>
       <c r="B44" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -3935,7 +3985,7 @@
         <v>238</v>
       </c>
       <c r="B45" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -3943,7 +3993,7 @@
         <v>239</v>
       </c>
       <c r="B46" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -3951,7 +4001,7 @@
         <v>24</v>
       </c>
       <c r="B47" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -3959,7 +4009,7 @@
         <v>242</v>
       </c>
       <c r="B48" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -3967,7 +4017,7 @@
         <v>246</v>
       </c>
       <c r="B49" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -3975,7 +4025,7 @@
         <v>249</v>
       </c>
       <c r="B50" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -3983,7 +4033,7 @@
         <v>250</v>
       </c>
       <c r="B51" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -3991,7 +4041,7 @@
         <v>254</v>
       </c>
       <c r="B52" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -3999,7 +4049,7 @@
         <v>258</v>
       </c>
       <c r="B53" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -4007,7 +4057,7 @@
         <v>260</v>
       </c>
       <c r="B54" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -4015,7 +4065,7 @@
         <v>262</v>
       </c>
       <c r="B55" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -4023,7 +4073,7 @@
         <v>266</v>
       </c>
       <c r="B56" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -4031,7 +4081,7 @@
         <v>268</v>
       </c>
       <c r="B57" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -4039,7 +4089,7 @@
         <v>270</v>
       </c>
       <c r="B58" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -4047,7 +4097,7 @@
         <v>276</v>
       </c>
       <c r="B59" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -4055,7 +4105,7 @@
         <v>28</v>
       </c>
       <c r="B60" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -4063,7 +4113,7 @@
         <v>288</v>
       </c>
       <c r="B61" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
@@ -4071,7 +4121,7 @@
         <v>292</v>
       </c>
       <c r="B62" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -4079,7 +4129,7 @@
         <v>296</v>
       </c>
       <c r="B63" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -4087,7 +4137,7 @@
         <v>300</v>
       </c>
       <c r="B64" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -4095,7 +4145,7 @@
         <v>304</v>
       </c>
       <c r="B65" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
@@ -4103,7 +4153,7 @@
         <v>308</v>
       </c>
       <c r="B66" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
@@ -4111,7 +4161,7 @@
         <v>31</v>
       </c>
       <c r="B67" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
@@ -4119,7 +4169,7 @@
         <v>312</v>
       </c>
       <c r="B68" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
@@ -4127,7 +4177,7 @@
         <v>316</v>
       </c>
       <c r="B69" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
@@ -4135,7 +4185,7 @@
         <v>32</v>
       </c>
       <c r="B70" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
@@ -4143,7 +4193,7 @@
         <v>320</v>
       </c>
       <c r="B71" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
@@ -4151,7 +4201,7 @@
         <v>324</v>
       </c>
       <c r="B72" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
@@ -4159,7 +4209,7 @@
         <v>328</v>
       </c>
       <c r="B73" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
@@ -4167,7 +4217,7 @@
         <v>332</v>
       </c>
       <c r="B74" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
@@ -4175,7 +4225,7 @@
         <v>334</v>
       </c>
       <c r="B75" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
@@ -4183,7 +4233,7 @@
         <v>336</v>
       </c>
       <c r="B76" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
@@ -4191,7 +4241,7 @@
         <v>340</v>
       </c>
       <c r="B77" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
@@ -4199,7 +4249,7 @@
         <v>344</v>
       </c>
       <c r="B78" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
@@ -4207,7 +4257,7 @@
         <v>348</v>
       </c>
       <c r="B79" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
@@ -4215,7 +4265,7 @@
         <v>352</v>
       </c>
       <c r="B80" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
@@ -4223,7 +4273,7 @@
         <v>356</v>
       </c>
       <c r="B81" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
@@ -4231,7 +4281,7 @@
         <v>36</v>
       </c>
       <c r="B82" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
@@ -4239,7 +4289,7 @@
         <v>360</v>
       </c>
       <c r="B83" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
@@ -4247,7 +4297,7 @@
         <v>364</v>
       </c>
       <c r="B84" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
@@ -4255,7 +4305,7 @@
         <v>368</v>
       </c>
       <c r="B85" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
@@ -4263,7 +4313,7 @@
         <v>372</v>
       </c>
       <c r="B86" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
@@ -4271,7 +4321,7 @@
         <v>376</v>
       </c>
       <c r="B87" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
@@ -4279,7 +4329,7 @@
         <v>380</v>
       </c>
       <c r="B88" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
@@ -4287,7 +4337,7 @@
         <v>384</v>
       </c>
       <c r="B89" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
@@ -4295,7 +4345,7 @@
         <v>388</v>
       </c>
       <c r="B90" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
@@ -4303,7 +4353,7 @@
         <v>392</v>
       </c>
       <c r="B91" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
@@ -4311,7 +4361,7 @@
         <v>398</v>
       </c>
       <c r="B92" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
@@ -4319,7 +4369,7 @@
         <v>4</v>
       </c>
       <c r="B93" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
@@ -4327,7 +4377,7 @@
         <v>40</v>
       </c>
       <c r="B94" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
@@ -4335,7 +4385,7 @@
         <v>400</v>
       </c>
       <c r="B95" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
@@ -4343,7 +4393,7 @@
         <v>404</v>
       </c>
       <c r="B96" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
@@ -4351,7 +4401,7 @@
         <v>408</v>
       </c>
       <c r="B97" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
@@ -4359,7 +4409,7 @@
         <v>410</v>
       </c>
       <c r="B98" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
@@ -4367,7 +4417,7 @@
         <v>414</v>
       </c>
       <c r="B99" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
@@ -4375,7 +4425,7 @@
         <v>417</v>
       </c>
       <c r="B100" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
@@ -4383,7 +4433,7 @@
         <v>418</v>
       </c>
       <c r="B101" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
@@ -4391,7 +4441,7 @@
         <v>422</v>
       </c>
       <c r="B102" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
@@ -4399,7 +4449,7 @@
         <v>426</v>
       </c>
       <c r="B103" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
@@ -4407,7 +4457,7 @@
         <v>428</v>
       </c>
       <c r="B104" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
@@ -4415,7 +4465,7 @@
         <v>430</v>
       </c>
       <c r="B105" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
@@ -4423,7 +4473,7 @@
         <v>434</v>
       </c>
       <c r="B106" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
@@ -4431,7 +4481,7 @@
         <v>438</v>
       </c>
       <c r="B107" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
@@ -4439,7 +4489,7 @@
         <v>44</v>
       </c>
       <c r="B108" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
@@ -4447,7 +4497,7 @@
         <v>440</v>
       </c>
       <c r="B109" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
@@ -4455,7 +4505,7 @@
         <v>442</v>
       </c>
       <c r="B110" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
@@ -4463,7 +4513,7 @@
         <v>446</v>
       </c>
       <c r="B111" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
@@ -4471,7 +4521,7 @@
         <v>450</v>
       </c>
       <c r="B112" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
@@ -4479,7 +4529,7 @@
         <v>454</v>
       </c>
       <c r="B113" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
@@ -4487,7 +4537,7 @@
         <v>458</v>
       </c>
       <c r="B114" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
@@ -4495,7 +4545,7 @@
         <v>462</v>
       </c>
       <c r="B115" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
@@ -4503,7 +4553,7 @@
         <v>466</v>
       </c>
       <c r="B116" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
@@ -4511,7 +4561,7 @@
         <v>470</v>
       </c>
       <c r="B117" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
@@ -4519,7 +4569,7 @@
         <v>474</v>
       </c>
       <c r="B118" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
@@ -4527,7 +4577,7 @@
         <v>478</v>
       </c>
       <c r="B119" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
@@ -4535,7 +4585,7 @@
         <v>48</v>
       </c>
       <c r="B120" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
@@ -4543,7 +4593,7 @@
         <v>480</v>
       </c>
       <c r="B121" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
@@ -4551,7 +4601,7 @@
         <v>484</v>
       </c>
       <c r="B122" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
@@ -4559,7 +4609,7 @@
         <v>492</v>
       </c>
       <c r="B123" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
@@ -4567,7 +4617,7 @@
         <v>496</v>
       </c>
       <c r="B124" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
@@ -4575,7 +4625,7 @@
         <v>498</v>
       </c>
       <c r="B125" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
@@ -4583,7 +4633,7 @@
         <v>50</v>
       </c>
       <c r="B126" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
@@ -4591,7 +4641,7 @@
         <v>500</v>
       </c>
       <c r="B127" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
@@ -4599,7 +4649,7 @@
         <v>504</v>
       </c>
       <c r="B128" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
@@ -4607,7 +4657,7 @@
         <v>508</v>
       </c>
       <c r="B129" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
@@ -4615,7 +4665,7 @@
         <v>51</v>
       </c>
       <c r="B130" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
@@ -4623,7 +4673,7 @@
         <v>512</v>
       </c>
       <c r="B131" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
@@ -4631,7 +4681,7 @@
         <v>516</v>
       </c>
       <c r="B132" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
@@ -4639,7 +4689,7 @@
         <v>52</v>
       </c>
       <c r="B133" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
@@ -4647,7 +4697,7 @@
         <v>520</v>
       </c>
       <c r="B134" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
@@ -4655,7 +4705,7 @@
         <v>524</v>
       </c>
       <c r="B135" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
@@ -4663,7 +4713,7 @@
         <v>528</v>
       </c>
       <c r="B136" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
@@ -4671,7 +4721,7 @@
         <v>530</v>
       </c>
       <c r="B137" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
@@ -4679,7 +4729,7 @@
         <v>533</v>
       </c>
       <c r="B138" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
@@ -4687,7 +4737,7 @@
         <v>540</v>
       </c>
       <c r="B139" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
@@ -4695,7 +4745,7 @@
         <v>548</v>
       </c>
       <c r="B140" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
@@ -4703,7 +4753,7 @@
         <v>554</v>
       </c>
       <c r="B141" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
@@ -4711,7 +4761,7 @@
         <v>558</v>
       </c>
       <c r="B142" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
@@ -4719,7 +4769,7 @@
         <v>56</v>
       </c>
       <c r="B143" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
@@ -4727,7 +4777,7 @@
         <v>562</v>
       </c>
       <c r="B144" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
@@ -4735,7 +4785,7 @@
         <v>566</v>
       </c>
       <c r="B145" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
@@ -4743,7 +4793,7 @@
         <v>570</v>
       </c>
       <c r="B146" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
@@ -4751,7 +4801,7 @@
         <v>574</v>
       </c>
       <c r="B147" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
@@ -4759,7 +4809,7 @@
         <v>578</v>
       </c>
       <c r="B148" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
@@ -4767,7 +4817,7 @@
         <v>580</v>
       </c>
       <c r="B149" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
@@ -4775,7 +4825,7 @@
         <v>581</v>
       </c>
       <c r="B150" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
@@ -4783,7 +4833,7 @@
         <v>583</v>
       </c>
       <c r="B151" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
@@ -4791,7 +4841,7 @@
         <v>584</v>
       </c>
       <c r="B152" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
@@ -4799,7 +4849,7 @@
         <v>585</v>
       </c>
       <c r="B153" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
@@ -4807,7 +4857,7 @@
         <v>586</v>
       </c>
       <c r="B154" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
@@ -4815,7 +4865,7 @@
         <v>591</v>
       </c>
       <c r="B155" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
@@ -4823,7 +4873,7 @@
         <v>598</v>
       </c>
       <c r="B156" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
@@ -4831,7 +4881,7 @@
         <v>60</v>
       </c>
       <c r="B157" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
@@ -4839,7 +4889,7 @@
         <v>600</v>
       </c>
       <c r="B158" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
@@ -4847,7 +4897,7 @@
         <v>604</v>
       </c>
       <c r="B159" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
@@ -4855,7 +4905,7 @@
         <v>608</v>
       </c>
       <c r="B160" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
@@ -4863,7 +4913,7 @@
         <v>612</v>
       </c>
       <c r="B161" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
@@ -4871,7 +4921,7 @@
         <v>616</v>
       </c>
       <c r="B162" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
@@ -4879,7 +4929,7 @@
         <v>620</v>
       </c>
       <c r="B163" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
@@ -4887,7 +4937,7 @@
         <v>624</v>
       </c>
       <c r="B164" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
@@ -4895,7 +4945,7 @@
         <v>626</v>
       </c>
       <c r="B165" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
@@ -4903,7 +4953,7 @@
         <v>630</v>
       </c>
       <c r="B166" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
@@ -4911,7 +4961,7 @@
         <v>634</v>
       </c>
       <c r="B167" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
@@ -4919,7 +4969,7 @@
         <v>638</v>
       </c>
       <c r="B168" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
@@ -4927,7 +4977,7 @@
         <v>64</v>
       </c>
       <c r="B169" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
@@ -4935,7 +4985,7 @@
         <v>642</v>
       </c>
       <c r="B170" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
@@ -4943,7 +4993,7 @@
         <v>643</v>
       </c>
       <c r="B171" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
@@ -4951,7 +5001,7 @@
         <v>646</v>
       </c>
       <c r="B172" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
@@ -4959,7 +5009,7 @@
         <v>654</v>
       </c>
       <c r="B173" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
@@ -4967,7 +5017,7 @@
         <v>659</v>
       </c>
       <c r="B174" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
@@ -4975,7 +5025,7 @@
         <v>660</v>
       </c>
       <c r="B175" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
@@ -4983,7 +5033,7 @@
         <v>662</v>
       </c>
       <c r="B176" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
@@ -4991,7 +5041,7 @@
         <v>666</v>
       </c>
       <c r="B177" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
@@ -4999,7 +5049,7 @@
         <v>670</v>
       </c>
       <c r="B178" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
@@ -5007,7 +5057,7 @@
         <v>674</v>
       </c>
       <c r="B179" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
@@ -5015,7 +5065,7 @@
         <v>678</v>
       </c>
       <c r="B180" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
@@ -5023,7 +5073,7 @@
         <v>68</v>
       </c>
       <c r="B181" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
@@ -5031,7 +5081,7 @@
         <v>682</v>
       </c>
       <c r="B182" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
@@ -5039,7 +5089,7 @@
         <v>686</v>
       </c>
       <c r="B183" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
@@ -5047,7 +5097,7 @@
         <v>690</v>
       </c>
       <c r="B184" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
@@ -5055,7 +5105,7 @@
         <v>694</v>
       </c>
       <c r="B185" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
@@ -5063,7 +5113,7 @@
         <v>70</v>
       </c>
       <c r="B186" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
@@ -5071,7 +5121,7 @@
         <v>702</v>
       </c>
       <c r="B187" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
@@ -5079,7 +5129,7 @@
         <v>703</v>
       </c>
       <c r="B188" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
@@ -5087,7 +5137,7 @@
         <v>704</v>
       </c>
       <c r="B189" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
@@ -5095,7 +5145,7 @@
         <v>705</v>
       </c>
       <c r="B190" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
@@ -5103,7 +5153,7 @@
         <v>706</v>
       </c>
       <c r="B191" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
@@ -5111,7 +5161,7 @@
         <v>710</v>
       </c>
       <c r="B192" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
@@ -5119,7 +5169,7 @@
         <v>716</v>
       </c>
       <c r="B193" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
@@ -5127,7 +5177,7 @@
         <v>72</v>
       </c>
       <c r="B194" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
@@ -5135,7 +5185,7 @@
         <v>724</v>
       </c>
       <c r="B195" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
@@ -5143,7 +5193,7 @@
         <v>732</v>
       </c>
       <c r="B196" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
@@ -5151,7 +5201,7 @@
         <v>736</v>
       </c>
       <c r="B197" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
@@ -5159,7 +5209,7 @@
         <v>74</v>
       </c>
       <c r="B198" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
@@ -5167,7 +5217,7 @@
         <v>740</v>
       </c>
       <c r="B199" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
@@ -5175,7 +5225,7 @@
         <v>744</v>
       </c>
       <c r="B200" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
@@ -5183,7 +5233,7 @@
         <v>748</v>
       </c>
       <c r="B201" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
@@ -5191,7 +5241,7 @@
         <v>752</v>
       </c>
       <c r="B202" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
@@ -5199,7 +5249,7 @@
         <v>756</v>
       </c>
       <c r="B203" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
@@ -5207,7 +5257,7 @@
         <v>76</v>
       </c>
       <c r="B204" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
@@ -5215,7 +5265,7 @@
         <v>760</v>
       </c>
       <c r="B205" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
@@ -5223,7 +5273,7 @@
         <v>762</v>
       </c>
       <c r="B206" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
@@ -5231,7 +5281,7 @@
         <v>764</v>
       </c>
       <c r="B207" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
@@ -5239,7 +5289,7 @@
         <v>768</v>
       </c>
       <c r="B208" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.25">
@@ -5247,7 +5297,7 @@
         <v>772</v>
       </c>
       <c r="B209" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.25">
@@ -5255,7 +5305,7 @@
         <v>776</v>
       </c>
       <c r="B210" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
@@ -5263,7 +5313,7 @@
         <v>780</v>
       </c>
       <c r="B211" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.25">
@@ -5271,7 +5321,7 @@
         <v>784</v>
       </c>
       <c r="B212" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.25">
@@ -5279,7 +5329,7 @@
         <v>788</v>
       </c>
       <c r="B213" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.25">
@@ -5287,7 +5337,7 @@
         <v>792</v>
       </c>
       <c r="B214" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.25">
@@ -5295,7 +5345,7 @@
         <v>795</v>
       </c>
       <c r="B215" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.25">
@@ -5303,7 +5353,7 @@
         <v>796</v>
       </c>
       <c r="B216" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.25">
@@ -5311,7 +5361,7 @@
         <v>798</v>
       </c>
       <c r="B217" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.25">
@@ -5319,7 +5369,7 @@
         <v>8</v>
       </c>
       <c r="B218" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.25">
@@ -5327,7 +5377,7 @@
         <v>800</v>
       </c>
       <c r="B219" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
@@ -5335,7 +5385,7 @@
         <v>804</v>
       </c>
       <c r="B220" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.25">
@@ -5343,7 +5393,7 @@
         <v>807</v>
       </c>
       <c r="B221" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.25">
@@ -5351,7 +5401,7 @@
         <v>818</v>
       </c>
       <c r="B222" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.25">
@@ -5359,7 +5409,7 @@
         <v>826</v>
       </c>
       <c r="B223" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.25">
@@ -5367,7 +5417,7 @@
         <v>834</v>
       </c>
       <c r="B224" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.25">
@@ -5375,7 +5425,7 @@
         <v>84</v>
       </c>
       <c r="B225" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.25">
@@ -5383,7 +5433,7 @@
         <v>840</v>
       </c>
       <c r="B226" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.25">
@@ -5391,7 +5441,7 @@
         <v>850</v>
       </c>
       <c r="B227" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.25">
@@ -5399,7 +5449,7 @@
         <v>854</v>
       </c>
       <c r="B228" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.25">
@@ -5407,7 +5457,7 @@
         <v>858</v>
       </c>
       <c r="B229" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.25">
@@ -5415,7 +5465,7 @@
         <v>86</v>
       </c>
       <c r="B230" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.25">
@@ -5423,7 +5473,7 @@
         <v>860</v>
       </c>
       <c r="B231" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.25">
@@ -5431,7 +5481,7 @@
         <v>862</v>
       </c>
       <c r="B232" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.25">
@@ -5439,7 +5489,7 @@
         <v>876</v>
       </c>
       <c r="B233" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.25">
@@ -5447,7 +5497,7 @@
         <v>882</v>
       </c>
       <c r="B234" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.25">
@@ -5455,7 +5505,7 @@
         <v>887</v>
       </c>
       <c r="B235" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.25">
@@ -5463,7 +5513,7 @@
         <v>891</v>
       </c>
       <c r="B236" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.25">
@@ -5471,7 +5521,7 @@
         <v>894</v>
       </c>
       <c r="B237" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.25">
@@ -5479,7 +5529,7 @@
         <v>90</v>
       </c>
       <c r="B238" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.25">
@@ -5487,7 +5537,7 @@
         <v>92</v>
       </c>
       <c r="B239" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.25">
@@ -5495,7 +5545,7 @@
         <v>96</v>
       </c>
       <c r="B240" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
   </sheetData>
@@ -5519,10 +5569,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="B1" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -5530,7 +5580,7 @@
         <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -5538,7 +5588,7 @@
         <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
     </row>
   </sheetData>
@@ -5562,10 +5612,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="B1" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -5573,7 +5623,7 @@
         <v>50</v>
       </c>
       <c r="B2" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -5581,7 +5631,7 @@
         <v>51</v>
       </c>
       <c r="B3" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -5589,7 +5639,7 @@
         <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -5597,7 +5647,7 @@
         <v>53</v>
       </c>
       <c r="B5" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -5605,7 +5655,7 @@
         <v>54</v>
       </c>
       <c r="B6" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
     </row>
   </sheetData>
@@ -5629,10 +5679,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="B1" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -5640,7 +5690,7 @@
         <v>57</v>
       </c>
       <c r="B2" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -5648,7 +5698,7 @@
         <v>58</v>
       </c>
       <c r="B3" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -5656,7 +5706,7 @@
         <v>59</v>
       </c>
       <c r="B4" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -5664,7 +5714,7 @@
         <v>60</v>
       </c>
       <c r="B5" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -5672,7 +5722,7 @@
         <v>61</v>
       </c>
       <c r="B6" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -5680,7 +5730,7 @@
         <v>62</v>
       </c>
       <c r="B7" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -5688,7 +5738,7 @@
         <v>63</v>
       </c>
       <c r="B8" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -5696,7 +5746,7 @@
         <v>64</v>
       </c>
       <c r="B9" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -5704,7 +5754,7 @@
         <v>180</v>
       </c>
       <c r="B10" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
     </row>
   </sheetData>
@@ -5727,10 +5777,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="B1" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -5738,7 +5788,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -5746,7 +5796,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -5754,7 +5804,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -5762,7 +5812,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -5770,7 +5820,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -5778,7 +5828,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -5786,7 +5836,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -5794,7 +5844,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -5802,7 +5852,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -5810,7 +5860,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -5818,7 +5868,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -5826,7 +5876,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -5834,7 +5884,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -5842,7 +5892,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -5850,7 +5900,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -5858,7 +5908,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -5866,7 +5916,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -5874,7 +5924,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -5882,7 +5932,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -5890,7 +5940,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -5898,7 +5948,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -5906,7 +5956,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -5914,7 +5964,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -5922,7 +5972,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -5930,7 +5980,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -5938,7 +5988,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -5946,7 +5996,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -5954,7 +6004,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -5962,7 +6012,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -5970,7 +6020,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -5978,7 +6028,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -5986,7 +6036,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
     </row>
   </sheetData>
@@ -6009,10 +6059,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="B1" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -6020,7 +6070,7 @@
         <v>181</v>
       </c>
       <c r="B2" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -6028,7 +6078,7 @@
         <v>182</v>
       </c>
       <c r="B3" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -6036,7 +6086,7 @@
         <v>183</v>
       </c>
       <c r="B4" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -6044,7 +6094,7 @@
         <v>184</v>
       </c>
       <c r="B5" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -6052,7 +6102,7 @@
         <v>185</v>
       </c>
       <c r="B6" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -6060,7 +6110,7 @@
         <v>186</v>
       </c>
       <c r="B7" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -6068,7 +6118,7 @@
         <v>187</v>
       </c>
       <c r="B8" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -6076,7 +6126,7 @@
         <v>188</v>
       </c>
       <c r="B9" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -6084,7 +6134,7 @@
         <v>189</v>
       </c>
       <c r="B10" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -6092,7 +6142,7 @@
         <v>190</v>
       </c>
       <c r="B11" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -6100,7 +6150,7 @@
         <v>191</v>
       </c>
       <c r="B12" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -6108,7 +6158,7 @@
         <v>192</v>
       </c>
       <c r="B13" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -6116,7 +6166,7 @@
         <v>193</v>
       </c>
       <c r="B14" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -6124,7 +6174,7 @@
         <v>194</v>
       </c>
       <c r="B15" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -6132,7 +6182,7 @@
         <v>195</v>
       </c>
       <c r="B16" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -6140,7 +6190,7 @@
         <v>196</v>
       </c>
       <c r="B17" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -6148,7 +6198,7 @@
         <v>197</v>
       </c>
       <c r="B18" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -6156,7 +6206,7 @@
         <v>198</v>
       </c>
       <c r="B19" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -6164,7 +6214,7 @@
         <v>199</v>
       </c>
       <c r="B20" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
     </row>
   </sheetData>
@@ -6184,10 +6234,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="B1" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -6195,7 +6245,7 @@
         <v>69</v>
       </c>
       <c r="B2" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -6203,7 +6253,7 @@
         <v>70</v>
       </c>
       <c r="B3" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -6211,7 +6261,7 @@
         <v>71</v>
       </c>
       <c r="B4" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
     </row>
   </sheetData>
@@ -6235,10 +6285,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="B1" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -6246,7 +6296,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -6254,7 +6304,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -6262,7 +6312,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dispersion especial, campo retroactivo y ocultacion de campo de transporte, reporte de movimientos de posicion y sueldo
</commit_message>
<xml_diff>
--- a/Payroll/Content/Download/CargaMasiva.xlsx
+++ b/Payroll/Content/Download/CargaMasiva.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marco Carranza\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marco Carranza\Documents\IPSNET-Nomina\developeraguilar\Seri\Payroll\Content\Download\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7063EDA7-32A2-4112-930D-44188EA3FBF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ACF8760-43B7-4B4B-9398-17D14F6E9294}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{B7450375-384B-4A8B-AB27-614585F29454}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="13" activeTab="15" xr2:uid="{B7450375-384B-4A8B-AB27-614585F29454}"/>
   </bookViews>
   <sheets>
     <sheet name="IPSNet Cargas" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="513">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="514">
   <si>
     <t>DATA</t>
   </si>
@@ -1579,6 +1579,9 @@
   </si>
   <si>
     <t>28-08-1997</t>
+  </si>
+  <si>
+    <t>Retroactivo</t>
   </si>
 </sst>
 </file>
@@ -1984,10 +1987,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A634B92-38F3-48BB-89EF-6C7BAE71E424}">
-  <dimension ref="A1:AW7"/>
+  <dimension ref="A1:AX7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AJ1" workbookViewId="0">
-      <selection activeCell="AU9" sqref="AU9"/>
+    <sheetView topLeftCell="AJ1" workbookViewId="0">
+      <selection activeCell="AV7" sqref="AV7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2011,7 +2014,7 @@
     <col min="44" max="44" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A1" s="2">
         <v>2</v>
       </c>
@@ -2159,8 +2162,11 @@
       <c r="AW1" s="7" t="s">
         <v>507</v>
       </c>
-    </row>
-    <row r="2" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="AX1" s="7" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="2" spans="1:50" x14ac:dyDescent="0.25">
       <c r="D2">
         <v>18</v>
       </c>
@@ -2293,8 +2299,11 @@
       <c r="AW2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="AX2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:50" x14ac:dyDescent="0.25">
       <c r="D3">
         <v>18</v>
       </c>
@@ -2424,8 +2433,11 @@
       <c r="AV3" t="s">
         <v>508</v>
       </c>
-    </row>
-    <row r="7" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="AX3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:50" x14ac:dyDescent="0.25">
       <c r="H7" s="8"/>
       <c r="AB7" t="s">
         <v>49</v>
@@ -2843,7 +2855,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00E05364-4ABD-4239-B4EA-F0FE2D369467}">
   <dimension ref="A1:B95"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D1" activeCellId="1" sqref="C1:C1048576 D1:D1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Numero de nomina por carga masiva y modificacion archivos de dispersion
</commit_message>
<xml_diff>
--- a/Payroll/Content/Download/CargaMasiva.xlsx
+++ b/Payroll/Content/Download/CargaMasiva.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marco Carranza\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{985E0BC0-71A9-4175-BE07-2D2422E6F36C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="13" activeTab="16" xr2:uid="{B7450375-384B-4A8B-AB27-614585F29454}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310"/>
   </bookViews>
   <sheets>
     <sheet name="IPSNet Cargas" sheetId="1" r:id="rId1"/>
@@ -31,7 +30,7 @@
     <sheet name="CatalogoBancos" sheetId="16" r:id="rId16"/>
     <sheet name="CatalogoTipoSalario" sheetId="17" r:id="rId17"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="517">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="518">
   <si>
     <t>DATA</t>
   </si>
@@ -1592,13 +1591,16 @@
   </si>
   <si>
     <t>Tipo de Sueldo Mixto</t>
+  </si>
+  <si>
+    <t>NOMINA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1621,8 +1623,17 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1653,6 +1664,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1668,7 +1685,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -1681,6 +1698,9 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1996,11 +2016,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A634B92-38F3-48BB-89EF-6C7BAE71E424}">
-  <dimension ref="A1:AX7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AY7"/>
   <sheetViews>
-    <sheetView topLeftCell="AJ1" workbookViewId="0">
-      <selection activeCell="AV7" sqref="AV7"/>
+    <sheetView tabSelected="1" topLeftCell="AK1" workbookViewId="0">
+      <selection activeCell="AY2" sqref="AY2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2024,7 +2044,7 @@
     <col min="44" max="44" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A1" s="2">
         <v>2</v>
       </c>
@@ -2175,10 +2195,13 @@
       <c r="AX1" s="7" t="s">
         <v>513</v>
       </c>
-    </row>
-    <row r="2" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="AY1" s="10" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="2" spans="1:51" x14ac:dyDescent="0.25">
       <c r="D2">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="E2" t="s">
         <v>509</v>
@@ -2312,10 +2335,13 @@
       <c r="AX2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="AY2">
+        <v>10999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:51" x14ac:dyDescent="0.25">
       <c r="D3">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="E3" t="s">
         <v>2</v>
@@ -2446,8 +2472,11 @@
       <c r="AX3">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="AY3">
+        <v>10001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:51" x14ac:dyDescent="0.25">
       <c r="H7" s="8"/>
       <c r="AB7" t="s">
         <v>49</v>
@@ -2455,14 +2484,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="V2" r:id="rId1" xr:uid="{3DCF0280-088D-41B8-8FB9-724CDF55A9BF}"/>
+    <hyperlink ref="V2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2D2C3B7-668E-4202-BB63-B1E159CA56A9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2525,7 +2555,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45E09398-2C12-4ACC-9087-987AA781AF0C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2572,7 +2602,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A4E3568-EE9D-4294-83EC-A076500FEFB8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2627,7 +2657,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{986B18E5-4538-48C5-A894-C04B03686389}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2741,7 +2771,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BADE241E-7062-4401-B134-4F41C106E064}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2804,7 +2834,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E97F535-40D1-4AEC-A99F-0BBD574A23F7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2862,7 +2892,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00E05364-4ABD-4239-B4EA-F0FE2D369467}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B95"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3637,10 +3667,10 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61355364-11CE-4327-B1B4-FC9015EBBCA1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -3679,7 +3709,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F21BD5A-5DE9-4E68-8A58-5F806B8C8F96}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B240"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5618,7 +5648,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4BDEAC7-4A09-48D4-907E-33A8B25AA310}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5661,7 +5691,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5A7E065-DD6C-41EF-BC00-45E576E03AB6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5728,7 +5758,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7B0860A-4C2D-4C1A-8611-B521CFD759D2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5827,7 +5857,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80FFB44C-D04A-4911-AB17-8958283FA53C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6109,7 +6139,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0C50ADC-E328-4FB4-8210-54195927F941}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6287,7 +6317,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{968ED694-18AF-494E-AE3D-6EF697AD9144}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6334,7 +6364,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5489808C-0225-40DB-B1DA-A965A417A362}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Reporte acumulados, reporte catalogos generales, clasif nueva hoja de calculo
</commit_message>
<xml_diff>
--- a/Payroll/Content/Download/CargaMasiva.xlsx
+++ b/Payroll/Content/Download/CargaMasiva.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marco Carranza\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marco Carranza\Documents\Proyectos-Raciti\IPSNET-Nomina\devaguilar\Seri\Payroll\Content\Download\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="518">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="519">
   <si>
     <t>DATA</t>
   </si>
@@ -1594,6 +1594,9 @@
   </si>
   <si>
     <t>NOMINA</t>
+  </si>
+  <si>
+    <t>CLASIF</t>
   </si>
 </sst>
 </file>
@@ -2017,10 +2020,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AY7"/>
+  <dimension ref="A1:AZ7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AK1" workbookViewId="0">
-      <selection activeCell="AY2" sqref="AY2"/>
+    <sheetView tabSelected="1" topLeftCell="AM1" workbookViewId="0">
+      <selection activeCell="AW7" sqref="AW7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2044,7 +2047,7 @@
     <col min="44" max="44" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A1" s="2">
         <v>2</v>
       </c>
@@ -2198,8 +2201,11 @@
       <c r="AY1" s="10" t="s">
         <v>517</v>
       </c>
-    </row>
-    <row r="2" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="AZ1" s="10" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="2" spans="1:52" x14ac:dyDescent="0.25">
       <c r="D2">
         <v>4</v>
       </c>
@@ -2338,8 +2344,11 @@
       <c r="AY2">
         <v>10999</v>
       </c>
-    </row>
-    <row r="3" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="AZ2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:52" x14ac:dyDescent="0.25">
       <c r="D3">
         <v>4</v>
       </c>
@@ -2475,8 +2484,11 @@
       <c r="AY3">
         <v>10001</v>
       </c>
-    </row>
-    <row r="7" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="AZ3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:52" x14ac:dyDescent="0.25">
       <c r="H7" s="8"/>
       <c r="AB7" t="s">
         <v>49</v>

</xml_diff>

<commit_message>
Modificacion layout carga masiva, bajas empleados, sueldos de empleados
</commit_message>
<xml_diff>
--- a/Payroll/Content/Download/CargaMasiva.xlsx
+++ b/Payroll/Content/Download/CargaMasiva.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="519">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="520">
   <si>
     <t>DATA</t>
   </si>
@@ -1597,6 +1597,9 @@
   </si>
   <si>
     <t>CLASIF</t>
+  </si>
+  <si>
+    <t>PRESTACIONES</t>
   </si>
 </sst>
 </file>
@@ -2020,10 +2023,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AZ7"/>
+  <dimension ref="A1:BA7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AM1" workbookViewId="0">
-      <selection activeCell="AW7" sqref="AW7"/>
+      <selection activeCell="BA2" sqref="BA2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2045,9 +2048,10 @@
     <col min="37" max="37" width="10.140625" customWidth="1"/>
     <col min="38" max="38" width="19" customWidth="1"/>
     <col min="44" max="44" width="21.7109375" customWidth="1"/>
+    <col min="53" max="53" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A1" s="2">
         <v>2</v>
       </c>
@@ -2204,8 +2208,11 @@
       <c r="AZ1" s="10" t="s">
         <v>518</v>
       </c>
-    </row>
-    <row r="2" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="BA1" s="10" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="2" spans="1:53" x14ac:dyDescent="0.25">
       <c r="D2">
         <v>4</v>
       </c>
@@ -2347,8 +2354,11 @@
       <c r="AZ2">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="BA2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:53" x14ac:dyDescent="0.25">
       <c r="D3">
         <v>4</v>
       </c>
@@ -2487,8 +2497,11 @@
       <c r="AZ3">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="BA3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:53" x14ac:dyDescent="0.25">
       <c r="H7" s="8"/>
       <c r="AB7" t="s">
         <v>49</v>

</xml_diff>

<commit_message>
Complemento especial, carga masiva, captura y edicion de empleados
</commit_message>
<xml_diff>
--- a/Payroll/Content/Download/CargaMasiva.xlsx
+++ b/Payroll/Content/Download/CargaMasiva.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="520">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="521">
   <si>
     <t>DATA</t>
   </si>
@@ -1600,6 +1600,9 @@
   </si>
   <si>
     <t>PRESTACIONES</t>
+  </si>
+  <si>
+    <t>COMPLEMENTO ESPECIAL</t>
   </si>
 </sst>
 </file>
@@ -2023,10 +2026,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BA7"/>
+  <dimension ref="A1:BB7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AM1" workbookViewId="0">
-      <selection activeCell="BA2" sqref="BA2"/>
+    <sheetView tabSelected="1" topLeftCell="AU1" workbookViewId="0">
+      <selection activeCell="BC3" sqref="BC3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2051,7 +2054,7 @@
     <col min="53" max="53" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A1" s="2">
         <v>2</v>
       </c>
@@ -2211,8 +2214,11 @@
       <c r="BA1" s="10" t="s">
         <v>519</v>
       </c>
-    </row>
-    <row r="2" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="BB1" s="10" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="2" spans="1:54" x14ac:dyDescent="0.25">
       <c r="D2">
         <v>4</v>
       </c>
@@ -2357,8 +2363,11 @@
       <c r="BA2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="BB2">
+        <v>400.32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:54" x14ac:dyDescent="0.25">
       <c r="D3">
         <v>4</v>
       </c>
@@ -2500,8 +2509,11 @@
       <c r="BA3">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="BB3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:54" x14ac:dyDescent="0.25">
       <c r="H7" s="8"/>
       <c r="AB7" t="s">
         <v>49</v>

</xml_diff>